<commit_message>
corrected W gen units
</commit_message>
<xml_diff>
--- a/data/comp_ME200_clean.xlsx
+++ b/data/comp_ME200_clean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boltm/Documents/Fellowship/NIH_F31/Workshop_Feedback/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boltm/Documents/core-me-data-science-activities-public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F26B5F11-3A0B-8A46-8DD9-FE2EA662B45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED85D15-EBD4-A44D-B961-627B186F076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16700" xr2:uid="{76D00F18-B353-964D-8DF7-ABD8D72EA01D}"/>
+    <workbookView xWindow="1640" yWindow="4660" windowWidth="27640" windowHeight="16700" xr2:uid="{76D00F18-B353-964D-8DF7-ABD8D72EA01D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>[kg/s]</t>
   </si>
   <si>
-    <t>[kW]</t>
-  </si>
-  <si>
     <t>[kJ/kg]</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>[-]</t>
+  </si>
+  <si>
+    <t>[W]</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,22 +746,22 @@
         <v>14</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>